<commit_message>
numFormat & cellFormat cleanup
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>11000</t>
   </si>
@@ -72,16 +72,24 @@
   </si>
   <si>
     <t>Header</t>
+  </si>
+  <si>
+    <t>Float, CurrencyIntFormat</t>
+  </si>
+  <si>
+    <t>Float, CurrencyFormat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="170" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="171" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -118,16 +126,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -408,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ID11"/>
+  <dimension ref="A1:ID13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1079,6 +1089,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="1:238" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="9">
+        <v>4.123456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:238" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="10">
+        <v>4.123456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
support for selecting sheet by name || id || nr
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nodejs\xlsx-extract\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20625" windowHeight="10890"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27980" windowHeight="15800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="HelloWorld" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
   <si>
     <t>11000</t>
   </si>
@@ -78,6 +77,9 @@
   </si>
   <si>
     <t>Float, CurrencyFormat</t>
+  </si>
+  <si>
+    <t>Weeeeeh</t>
   </si>
 </sst>
 </file>
@@ -88,8 +90,8 @@
     <numFmt numFmtId="164" formatCode="0.00000000000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="171" formatCode="#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -136,8 +138,8 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -198,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,7 +235,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,7 +412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,22 +422,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ID13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:238">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:238" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:238" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1025,7 +1027,7 @@
         <v>1385.4006416040108</v>
       </c>
     </row>
-    <row r="4" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:238">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1035,7 @@
         <v>40574</v>
       </c>
     </row>
-    <row r="5" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:238">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1041,7 +1043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:238">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +1051,7 @@
         <v>5.9420289855072497</v>
       </c>
     </row>
-    <row r="7" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:238">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1057,7 +1059,7 @@
         <v>5.9420289855072461</v>
       </c>
     </row>
-    <row r="8" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:238">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>5.9420289855072461</v>
       </c>
     </row>
-    <row r="9" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:238">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1073,7 +1075,7 @@
         <v>5.9420289855072497</v>
       </c>
     </row>
-    <row r="10" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:238">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1081,7 +1083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:238">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1089,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:238">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1097,7 +1099,7 @@
         <v>4.123456</v>
       </c>
     </row>
-    <row r="13" spans="1:238" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:238">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1108,5 +1110,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added handling for float based integer percent format snowflake
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ffalt/Projekte/own/xlsx-extract/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27980" windowHeight="15800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="15800"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -12,10 +17,13 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
   <si>
     <t>11000</t>
   </si>
@@ -80,18 +88,22 @@
   </si>
   <si>
     <t>Weeeeeh</t>
+  </si>
+  <si>
+    <t>Float, FormatPercent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.00000000000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="169" formatCode="0\ %"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -116,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -124,11 +136,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -140,9 +167,12 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -412,7 +442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,24 +450,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ID13"/>
+  <dimension ref="A1:ID14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:238">
+    <row r="1" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:238" s="1" customFormat="1">
+    <row r="3" spans="1:238" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1057,7 @@
         <v>1385.4006416040108</v>
       </c>
     </row>
-    <row r="4" spans="1:238">
+    <row r="4" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1065,7 @@
         <v>40574</v>
       </c>
     </row>
-    <row r="5" spans="1:238">
+    <row r="5" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1043,7 +1073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:238">
+    <row r="6" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1051,7 +1081,7 @@
         <v>5.9420289855072497</v>
       </c>
     </row>
-    <row r="7" spans="1:238">
+    <row r="7" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1059,7 +1089,7 @@
         <v>5.9420289855072461</v>
       </c>
     </row>
-    <row r="8" spans="1:238">
+    <row r="8" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1097,7 @@
         <v>5.9420289855072461</v>
       </c>
     </row>
-    <row r="9" spans="1:238">
+    <row r="9" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1075,7 +1105,7 @@
         <v>5.9420289855072497</v>
       </c>
     </row>
-    <row r="10" spans="1:238">
+    <row r="10" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1083,7 +1113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:238">
+    <row r="11" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1091,7 +1121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:238">
+    <row r="12" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1099,22 +1129,25 @@
         <v>4.123456</v>
       </c>
     </row>
-    <row r="13" spans="1:238">
+    <row r="13" spans="1:238" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="10">
         <v>4.123456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:238" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1122,23 +1155,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add test for issue with percent formatting
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ffalt/Projekte/own/xlsx-extract/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ffalt/Projekte/public/xlsx-extract/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3477BFBA-17DA-1548-8C80-DFBD56B905CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="15800"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="HelloWorld" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
   <si>
     <t>11000</t>
   </si>
@@ -91,12 +92,15 @@
   </si>
   <si>
     <t>Float, FormatPercent</t>
+  </si>
+  <si>
+    <t>Value with Percent Char</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.00000000000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -155,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -170,9 +174,10 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,11 +454,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ID14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:ID15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1145,6 +1150,14 @@
         <v>0.8</v>
       </c>
     </row>
+    <row r="15" spans="1:238" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1152,7 +1165,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>